<commit_message>
feat: ajustes del calculo de cantidad_real
</commit_message>
<xml_diff>
--- a/01_simulation/input/configuracion_hw.xlsx
+++ b/01_simulation/input/configuracion_hw.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c5d37b6e6ced8c36/Trabajo/Portafolio/telecom-hw-inventory-data-product/01_simulation/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="11_AD4D2F04E46CFB4ACB3E206A4D96EB04683EDF1E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{152E7927-B23A-4B90-AD73-3E64DE279CDC}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="11_AD4D2F04E46CFB4ACB3E206A4D96EB04683EDF1E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0D2C33E-8BAE-498C-87A6-19CCC293B66C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +599,7 @@
         <v>-3</v>
       </c>
       <c r="J2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -632,7 +632,7 @@
         <v>-3</v>
       </c>
       <c r="J3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -665,7 +665,7 @@
         <v>-3</v>
       </c>
       <c r="J4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -731,7 +731,7 @@
         <v>-3</v>
       </c>
       <c r="J6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -764,7 +764,7 @@
         <v>-4</v>
       </c>
       <c r="J7" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -797,7 +797,7 @@
         <v>-40</v>
       </c>
       <c r="J8" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -830,7 +830,7 @@
         <v>-60</v>
       </c>
       <c r="J9" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -863,7 +863,7 @@
         <v>-80</v>
       </c>
       <c r="J10" s="1">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -896,7 +896,7 @@
         <v>-30</v>
       </c>
       <c r="J11" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -929,7 +929,7 @@
         <v>-50</v>
       </c>
       <c r="J12" s="1">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -962,7 +962,7 @@
         <v>-70</v>
       </c>
       <c r="J13" s="1">
-        <v>15</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -995,7 +995,7 @@
         <v>-1</v>
       </c>
       <c r="J14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1028,7 +1028,7 @@
         <v>-1</v>
       </c>
       <c r="J15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1061,7 +1061,7 @@
         <v>-1</v>
       </c>
       <c r="J16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1094,7 +1094,7 @@
         <v>-6</v>
       </c>
       <c r="J17" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1127,7 +1127,7 @@
         <v>-8</v>
       </c>
       <c r="J18" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1160,7 +1160,7 @@
         <v>-12</v>
       </c>
       <c r="J19" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1193,7 +1193,7 @@
         <v>-3</v>
       </c>
       <c r="J20" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1226,7 +1226,7 @@
         <v>-6</v>
       </c>
       <c r="J21" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1259,7 +1259,7 @@
         <v>-3</v>
       </c>
       <c r="J22" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1292,7 +1292,7 @@
         <v>-3</v>
       </c>
       <c r="J23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1325,7 +1325,7 @@
         <v>-6</v>
       </c>
       <c r="J24" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1358,7 +1358,7 @@
         <v>-9</v>
       </c>
       <c r="J25" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1391,7 +1391,7 @@
         <v>-3</v>
       </c>
       <c r="J26" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -1424,7 +1424,7 @@
         <v>-3</v>
       </c>
       <c r="J27" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1457,7 +1457,7 @@
         <v>-3</v>
       </c>
       <c r="J28" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -1523,7 +1523,7 @@
         <v>-5</v>
       </c>
       <c r="J30" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -1556,7 +1556,7 @@
         <v>-7</v>
       </c>
       <c r="J31" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>